<commit_message>
update forecast, including 2018 run
</commit_message>
<xml_diff>
--- a/NSAS/results/stf/NSAS_stf_2020_tab.xlsx
+++ b/NSAS/results/stf/NSAS_stf_2020_tab.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\wg_HAWG\NSAS\results\stf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C4AB13BE-A6B1-40DF-A104-FE7CB48047D5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{02170B20-016B-4E0F-8408-A350FEEB7AFE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13725" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -267,7 +267,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -447,8 +447,14 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -563,6 +569,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -608,9 +629,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -968,8 +993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -984,52 +1009,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>34</v>
       </c>
       <c r="S1" t="s">
@@ -1040,1080 +1066,1083 @@
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="3">
         <v>0.18971109671771</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="3">
         <v>1.7852728050151801E-2</v>
       </c>
-      <c r="D2">
-        <v>2.2627225700794899E-11</v>
-      </c>
-      <c r="E2">
-        <v>1.90586722170282E-10</v>
-      </c>
-      <c r="F2">
+      <c r="D2" s="3">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3">
         <v>0.18981601755250199</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="3">
         <v>1.8612989801510001E-2</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="4">
         <v>379123.90926072001</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="4">
         <v>5614.9800130160002</v>
       </c>
-      <c r="J2">
-        <v>3.8399097254257398E-5</v>
-      </c>
-      <c r="K2">
-        <v>5.99426951850794E-5</v>
-      </c>
-      <c r="L2">
+      <c r="J2" s="1">
+        <v>0</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0</v>
+      </c>
+      <c r="L2" s="4">
         <f>SUM(H2:K2)</f>
-        <v>384738.88937207783</v>
-      </c>
-      <c r="M2">
+        <v>384738.88927373604</v>
+      </c>
+      <c r="M2" s="4">
         <v>1297964.88306625</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
       <c r="S2">
         <v>385008</v>
       </c>
       <c r="U2">
-        <v>418649</v>
+        <v>431062</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="3">
         <v>0.22181704827454199</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="3">
         <v>1.7852728050151801E-2</v>
       </c>
-      <c r="D3">
-        <v>5.6967825709623297E-8</v>
-      </c>
-      <c r="E3">
-        <v>3.0349571980291901E-7</v>
-      </c>
-      <c r="F3">
+      <c r="D3" s="3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3">
         <v>0.22192200672047599</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="3">
         <v>1.8742013691114601E-2</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="4">
         <v>365422.11410823499</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="4">
         <v>5882.3656761106504</v>
       </c>
-      <c r="J3">
-        <v>0.100000000000001</v>
-      </c>
-      <c r="K3">
-        <v>0.1</v>
-      </c>
-      <c r="L3">
+      <c r="J3" s="1">
+        <v>0</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0</v>
+      </c>
+      <c r="L3" s="4">
         <f t="shared" ref="L3:L20" si="0">SUM(H3:K3)</f>
-        <v>371304.67978434562</v>
-      </c>
-      <c r="M3">
+        <v>371304.47978434566</v>
+      </c>
+      <c r="M3" s="4">
         <v>1194964.6515718</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="4">
         <v>1185994.5596193699</v>
       </c>
-      <c r="O3">
+      <c r="O3" s="3">
         <f>(M3-$M$2)*100/$M$2</f>
         <v>-7.9355175812713208</v>
       </c>
-      <c r="P3">
+      <c r="P3" s="3">
         <f>(H3-$S$2)*100/$S$2</f>
         <v>-5.0871373820193364</v>
       </c>
-      <c r="Q3">
+      <c r="Q3" s="3">
         <f>(L3-$U$2)*100/$U$2</f>
-        <v>-11.30883394338799</v>
+        <v>-13.862859685069511</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="3">
         <v>0.21779818792893199</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="3">
         <v>1.78525402540128E-2</v>
       </c>
-      <c r="D4">
-        <v>8.6716139817565904E-9</v>
-      </c>
-      <c r="E4">
-        <v>1.1016059266796399E-8</v>
-      </c>
-      <c r="F4">
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0</v>
+      </c>
+      <c r="F4" s="3">
         <v>0.217903113165408</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="3">
         <v>1.8725379656635399E-2</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="4">
         <v>359837.45067426999</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="4">
         <v>5882.3666515391096</v>
       </c>
-      <c r="J4">
-        <v>1.52253361333392E-2</v>
-      </c>
-      <c r="K4">
-        <v>3.62976353731038E-3</v>
-      </c>
-      <c r="L4">
+      <c r="J4" s="1">
+        <v>0</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0</v>
+      </c>
+      <c r="L4" s="4">
         <f t="shared" si="0"/>
-        <v>365719.83618090878</v>
-      </c>
-      <c r="M4">
+        <v>365719.8173258091</v>
+      </c>
+      <c r="M4" s="4">
         <v>1198573.82186475</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="4">
         <v>1191992.4844736301</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="3">
         <f t="shared" ref="O4:O20" si="1">(M4-$M$2)*100/$M$2</f>
         <v>-7.6574537954141961</v>
       </c>
-      <c r="P4">
+      <c r="P4" s="3">
         <f t="shared" ref="P4:P20" si="2">(H4-$S$2)*100/$S$2</f>
         <v>-6.5376691719990259</v>
       </c>
-      <c r="Q4">
+      <c r="Q4" s="3">
         <f t="shared" ref="Q4:Q20" si="3">(L4-$U$2)*100/$U$2</f>
-        <v>-12.642849694873561</v>
+        <v>-15.158418666964591</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="3">
         <v>0.22181707471637299</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="3">
         <v>1.7852728050151801E-2</v>
       </c>
-      <c r="D5">
-        <v>1.7347084802367299E-8</v>
-      </c>
-      <c r="E5">
-        <v>1.10161751761508E-8</v>
-      </c>
-      <c r="F5">
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3">
         <v>0.22192200651493901</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="3">
         <v>1.8741681696794001E-2</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="4">
         <v>365422.15330593003</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="4">
         <v>5882.36663649207</v>
       </c>
-      <c r="J5">
-        <v>3.0450672266666898E-2</v>
-      </c>
-      <c r="K5">
-        <v>3.6297635373093899E-3</v>
-      </c>
-      <c r="L5">
+      <c r="J5" s="1">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0</v>
+      </c>
+      <c r="L5" s="4">
         <f t="shared" si="0"/>
-        <v>371304.55402285792</v>
-      </c>
-      <c r="M5">
+        <v>371304.51994242211</v>
+      </c>
+      <c r="M5" s="4">
         <v>1194964.65046505</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="4">
         <v>1185994.6358368699</v>
       </c>
-      <c r="O5">
+      <c r="O5" s="3">
         <f t="shared" si="1"/>
         <v>-7.9355176665394209</v>
       </c>
-      <c r="P5">
+      <c r="P5" s="3">
         <f t="shared" si="2"/>
         <v>-5.0871272010114001</v>
       </c>
-      <c r="Q5">
+      <c r="Q5" s="3">
         <f t="shared" si="3"/>
-        <v>-11.308863983227496</v>
+        <v>-13.862850368990514</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="3">
         <v>0.187751807871259</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="3">
         <v>4.0114451342223897E-2</v>
       </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3">
         <v>0.18798756125831501</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="3">
         <v>4.08668610889978E-2</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="4">
         <v>317015.27061757201</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="4">
         <v>13067.6949647089</v>
       </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
+      <c r="J6" s="1">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0</v>
+      </c>
+      <c r="L6" s="4">
         <f t="shared" si="0"/>
         <v>330082.96558228089</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="4">
         <v>1226005.83428234</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="4">
         <v>1236553.1542724799</v>
       </c>
-      <c r="O6">
+      <c r="O6" s="3">
         <f t="shared" si="1"/>
         <v>-5.5439904209054864</v>
       </c>
-      <c r="P6">
+      <c r="P6" s="3">
         <f t="shared" si="2"/>
         <v>-17.660082227493451</v>
       </c>
-      <c r="Q6">
+      <c r="Q6" s="3">
         <f t="shared" si="3"/>
-        <v>-21.155200279403299</v>
+        <v>-23.425640492021824</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="3">
         <v>0.187751807871259</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="3">
         <v>4.0114451342223897E-2</v>
       </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3">
         <v>0.18798756125831501</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="3">
         <v>4.08668610889978E-2</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="4">
         <v>317015.27061757201</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="4">
         <v>13067.6949647089</v>
       </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7">
+      <c r="J7" s="1">
+        <v>0</v>
+      </c>
+      <c r="K7" s="1">
+        <v>0</v>
+      </c>
+      <c r="L7" s="4">
         <f t="shared" si="0"/>
         <v>330082.96558228089</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="4">
         <v>1226005.83428234</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="4">
         <v>1236553.1542724799</v>
       </c>
-      <c r="O7">
+      <c r="O7" s="3">
         <f t="shared" si="1"/>
         <v>-5.5439904209054864</v>
       </c>
-      <c r="P7">
+      <c r="P7" s="3">
         <f t="shared" si="2"/>
         <v>-17.660082227493451</v>
       </c>
-      <c r="Q7">
+      <c r="Q7" s="3">
         <f t="shared" si="3"/>
-        <v>-21.155200279403299</v>
+        <v>-23.425640492021824</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="3">
         <v>0.187751807871259</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="3">
         <v>4.0114451342223897E-2</v>
       </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
+      <c r="D8" s="3">
+        <v>0</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0</v>
+      </c>
+      <c r="F8" s="3">
         <v>0.18798756125831501</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="3">
         <v>4.08668610889978E-2</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="4">
         <v>317015.27061757201</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="4">
         <v>13067.6949647089</v>
       </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
+      <c r="J8" s="1">
+        <v>0</v>
+      </c>
+      <c r="K8" s="1">
+        <v>0</v>
+      </c>
+      <c r="L8" s="4">
         <f t="shared" si="0"/>
         <v>330082.96558228089</v>
       </c>
-      <c r="M8">
+      <c r="M8" s="4">
         <v>1226005.83428234</v>
       </c>
-      <c r="N8">
+      <c r="N8" s="4">
         <v>1236553.1542724799</v>
       </c>
-      <c r="O8">
+      <c r="O8" s="3">
         <f t="shared" si="1"/>
         <v>-5.5439904209054864</v>
       </c>
-      <c r="P8">
+      <c r="P8" s="3">
         <f t="shared" si="2"/>
         <v>-17.660082227493451</v>
       </c>
-      <c r="Q8">
+      <c r="Q8" s="3">
         <f t="shared" si="3"/>
-        <v>-21.155200279403299</v>
+        <v>-23.425640492021824</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="3">
         <v>0.191772865490872</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="3">
         <v>4.92314759852484E-2</v>
       </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3">
         <v>0.19206219980369299</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="3">
         <v>0.05</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="4">
         <v>322848.82893140498</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="4">
         <v>15962.7127511822</v>
       </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9">
+      <c r="J9" s="1">
+        <v>0</v>
+      </c>
+      <c r="K9" s="1">
+        <v>0</v>
+      </c>
+      <c r="L9" s="4">
         <f t="shared" si="0"/>
         <v>338811.54168258718</v>
       </c>
-      <c r="M9">
+      <c r="M9" s="4">
         <v>1222213.99875077</v>
       </c>
-      <c r="N9">
+      <c r="N9" s="4">
         <v>1229184.5031472701</v>
       </c>
-      <c r="O9">
+      <c r="O9" s="3">
         <f t="shared" si="1"/>
         <v>-5.8361274102061804</v>
       </c>
-      <c r="P9">
+      <c r="P9" s="3">
         <f t="shared" si="2"/>
         <v>-16.144903760076421</v>
       </c>
-      <c r="Q9">
+      <c r="Q9" s="3">
         <f t="shared" si="3"/>
-        <v>-19.070261320918675</v>
+        <v>-21.400740106391385</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="3">
         <v>0.25990373921313498</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="3">
         <v>1.7852728050151801E-2</v>
       </c>
-      <c r="D10">
-        <v>5.7087625130457001E-8</v>
-      </c>
-      <c r="E10">
-        <v>3.0352564859059098E-7</v>
-      </c>
-      <c r="F10">
+      <c r="D10" s="3">
+        <v>0</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0</v>
+      </c>
+      <c r="F10" s="3">
         <v>0.26000869773462099</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="3">
         <v>1.88946451140619E-2</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="4">
         <v>416773.02872596902</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="4">
         <v>5881.7856979930102</v>
       </c>
-      <c r="J10">
-        <v>0.10000000010971501</v>
-      </c>
-      <c r="K10">
-        <v>0.100000000775176</v>
-      </c>
-      <c r="L10">
+      <c r="J10" s="1">
+        <v>0</v>
+      </c>
+      <c r="K10" s="1">
+        <v>0</v>
+      </c>
+      <c r="L10" s="4">
         <f t="shared" si="0"/>
-        <v>422655.01442396292</v>
-      </c>
-      <c r="M10">
+        <v>422654.81442396203</v>
+      </c>
+      <c r="M10" s="4">
         <v>1161612.8442795801</v>
       </c>
-      <c r="N10">
+      <c r="N10" s="4">
         <v>1131960.88206297</v>
       </c>
-      <c r="O10">
+      <c r="O10" s="3">
         <f t="shared" si="1"/>
         <v>-10.505063778348028</v>
       </c>
-      <c r="P10">
+      <c r="P10" s="3">
         <f t="shared" si="2"/>
         <v>8.2504853732828991</v>
       </c>
-      <c r="Q10">
+      <c r="Q10" s="3">
         <f t="shared" si="3"/>
-        <v>0.95689095733249463</v>
+        <v>-1.9503425437728144</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11">
+      <c r="B11" s="3">
+        <v>0</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0</v>
+      </c>
+      <c r="G11" s="3">
+        <v>0</v>
+      </c>
+      <c r="H11" s="4">
+        <v>0</v>
+      </c>
+      <c r="I11" s="4">
+        <v>0</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0</v>
+      </c>
+      <c r="K11" s="1">
+        <v>0</v>
+      </c>
+      <c r="L11" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M11">
+      <c r="M11" s="4">
         <v>1423553.23179569</v>
       </c>
-      <c r="N11">
+      <c r="N11" s="4">
         <v>1634511.7064158299</v>
       </c>
-      <c r="O11">
+      <c r="O11" s="3">
         <f t="shared" si="1"/>
         <v>9.675789412172394</v>
       </c>
-      <c r="P11">
+      <c r="P11" s="3">
         <f t="shared" si="2"/>
         <v>-100</v>
       </c>
-      <c r="Q11">
+      <c r="Q11" s="3">
         <f t="shared" si="3"/>
         <v>-100</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="3">
         <v>0.23609928629001101</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="3">
         <v>1.7852728050151801E-2</v>
       </c>
-      <c r="D12">
-        <v>5.7012796363845402E-8</v>
-      </c>
-      <c r="E12">
-        <v>3.0350694951822301E-7</v>
-      </c>
-      <c r="F12">
+      <c r="D12" s="3">
+        <v>0</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0</v>
+      </c>
+      <c r="F12" s="3">
         <v>0.23620424476430599</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="3">
         <v>1.87992493884011E-2</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="4">
         <v>385008.04999716103</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="4">
         <v>5882.14797418546</v>
       </c>
-      <c r="J12">
-        <v>0.100000000000008</v>
-      </c>
-      <c r="K12">
-        <v>9.9999999061467601E-2</v>
-      </c>
-      <c r="L12">
+      <c r="J12" s="1">
+        <v>0</v>
+      </c>
+      <c r="K12" s="1">
+        <v>0</v>
+      </c>
+      <c r="L12" s="4">
         <f t="shared" si="0"/>
-        <v>390890.39797134552</v>
-      </c>
-      <c r="M12">
+        <v>390890.1979713465</v>
+      </c>
+      <c r="M12" s="4">
         <v>1182278.96423635</v>
       </c>
-      <c r="N12">
+      <c r="N12" s="4">
         <v>1165149.24192006</v>
       </c>
-      <c r="O12">
+      <c r="O12" s="3">
         <f t="shared" si="1"/>
         <v>-8.9128697038866811</v>
       </c>
-      <c r="P12">
+      <c r="P12" s="3">
         <f t="shared" si="2"/>
         <v>1.298600575211755E-5</v>
       </c>
-      <c r="Q12">
+      <c r="Q12" s="3">
         <f t="shared" si="3"/>
-        <v>-6.6305191290686176</v>
+        <v>-9.3192631288894638</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+      <c r="A13" s="5">
         <v>-0.15</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="3">
         <v>0.19481112333456399</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="3">
         <v>1.7852728050151801E-2</v>
       </c>
-      <c r="D13">
-        <v>5.6882636402227998E-8</v>
-      </c>
-      <c r="E13">
-        <v>3.03474446278007E-7</v>
-      </c>
-      <c r="F13">
+      <c r="D13" s="3">
+        <v>0</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0</v>
+      </c>
+      <c r="F13" s="3">
         <v>0.19491608172677499</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="3">
         <v>1.8633788149297201E-2</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="4">
         <v>327256.84960990603</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="4">
         <v>5882.7780292859497</v>
       </c>
-      <c r="J13">
-        <v>9.9999999971131695E-2</v>
-      </c>
-      <c r="K13">
-        <v>9.9999999999932407E-2</v>
-      </c>
-      <c r="L13">
+      <c r="J13" s="1">
+        <v>0</v>
+      </c>
+      <c r="K13" s="1">
+        <v>0</v>
+      </c>
+      <c r="L13" s="4">
         <f t="shared" si="0"/>
-        <v>333139.82763919194</v>
-      </c>
-      <c r="M13">
+        <v>333139.62763919198</v>
+      </c>
+      <c r="M13" s="4">
         <v>1219557.9099800901</v>
       </c>
-      <c r="N13">
+      <c r="N13" s="4">
         <v>1227466.4524769201</v>
       </c>
-      <c r="O13">
+      <c r="O13" s="3">
         <f t="shared" si="1"/>
         <v>-6.0407622817140503</v>
       </c>
-      <c r="P13">
+      <c r="P13" s="3">
         <f t="shared" si="2"/>
         <v>-14.999987114577872</v>
       </c>
-      <c r="Q13">
+      <c r="Q13" s="3">
         <f t="shared" si="3"/>
-        <v>-20.42502725691643</v>
+        <v>-22.716540163783403</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
+      <c r="A14" s="5">
         <v>0.15</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="3">
         <v>0.27999361750339702</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="3">
         <v>1.7852728050151801E-2</v>
       </c>
-      <c r="D14">
-        <v>5.7150657295519902E-8</v>
-      </c>
-      <c r="E14">
-        <v>3.03541396249614E-7</v>
-      </c>
-      <c r="F14">
+      <c r="D14" s="3">
+        <v>0</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0</v>
+      </c>
+      <c r="F14" s="3">
         <v>0.28009857606463401</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="3">
         <v>1.8975154778387002E-2</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="4">
         <v>442759.24954855797</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="4">
         <v>5881.4805066923</v>
       </c>
-      <c r="J14">
-        <v>9.9999999999907899E-2</v>
-      </c>
-      <c r="K14">
-        <v>0.100000000000061</v>
-      </c>
-      <c r="L14">
+      <c r="J14" s="1">
+        <v>0</v>
+      </c>
+      <c r="K14" s="1">
+        <v>0</v>
+      </c>
+      <c r="L14" s="4">
         <f t="shared" si="0"/>
-        <v>448640.93005525024</v>
-      </c>
-      <c r="M14">
+        <v>448640.73005525029</v>
+      </c>
+      <c r="M14" s="4">
         <v>1144622.7695116899</v>
       </c>
-      <c r="N14">
+      <c r="N14" s="4">
         <v>1105370.1353086301</v>
       </c>
-      <c r="O14">
+      <c r="O14" s="3">
         <f t="shared" si="1"/>
         <v>-11.81404177841176</v>
       </c>
-      <c r="P14">
+      <c r="P14" s="3">
         <f t="shared" si="2"/>
         <v>15.000012869487898</v>
       </c>
-      <c r="Q14">
+      <c r="Q14" s="3">
         <f t="shared" si="3"/>
-        <v>7.1639798626654398</v>
+        <v>4.078005032976761</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="3">
         <v>0.18971574075929001</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="3">
         <v>1.7852728050151801E-2</v>
       </c>
-      <c r="D15">
-        <v>5.6866540242224299E-8</v>
-      </c>
-      <c r="E15">
-        <v>3.0347043011406598E-7</v>
-      </c>
-      <c r="F15">
+      <c r="D15" s="3">
+        <v>0</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0</v>
+      </c>
+      <c r="F15" s="3">
         <v>0.189820699141349</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="3">
         <v>1.8613368536124001E-2</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="4">
         <v>319884.71577490598</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="4">
         <v>5882.8559345601298</v>
       </c>
-      <c r="J15">
-        <v>0.100000000103929</v>
-      </c>
-      <c r="K15">
-        <v>0.10000000088193001</v>
-      </c>
-      <c r="L15">
+      <c r="J15" s="1">
+        <v>0</v>
+      </c>
+      <c r="K15" s="1">
+        <v>0</v>
+      </c>
+      <c r="L15" s="4">
         <f t="shared" si="0"/>
-        <v>325767.77170946711</v>
-      </c>
-      <c r="M15">
+        <v>325767.57170946611</v>
+      </c>
+      <c r="M15" s="4">
         <v>1224289.06767751</v>
       </c>
-      <c r="N15">
+      <c r="N15" s="4">
         <v>1235608.89392044</v>
       </c>
-      <c r="O15">
+      <c r="O15" s="3">
         <f t="shared" si="1"/>
         <v>-5.6762564496114738</v>
       </c>
-      <c r="P15">
+      <c r="P15" s="3">
         <f t="shared" si="2"/>
         <v>-16.91478728366528</v>
       </c>
-      <c r="Q15">
+      <c r="Q15" s="3">
         <f t="shared" si="3"/>
-        <v>-22.185942947560576</v>
+        <v>-24.426747959814108</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="3">
         <v>0.29990655684655998</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="3">
         <v>1.7852728050151801E-2</v>
       </c>
-      <c r="D16">
-        <v>5.7213027621327601E-8</v>
-      </c>
-      <c r="E16">
-        <v>3.0355698582305701E-7</v>
-      </c>
-      <c r="F16">
+      <c r="D16" s="3">
+        <v>0</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0</v>
+      </c>
+      <c r="F16" s="3">
         <v>0.30001151544713001</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="3">
         <v>1.9054955364361099E-2</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="4">
         <v>467805.53150954598</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="4">
         <v>5881.1785008607403</v>
       </c>
-      <c r="J16">
-        <v>0.100000000103282</v>
-      </c>
-      <c r="K16">
-        <v>0.100000000772625</v>
-      </c>
-      <c r="L16">
+      <c r="J16" s="1">
+        <v>0</v>
+      </c>
+      <c r="K16" s="1">
+        <v>0</v>
+      </c>
+      <c r="L16" s="4">
         <f t="shared" si="0"/>
-        <v>473686.91001040762</v>
-      </c>
-      <c r="M16">
+        <v>473686.71001040674</v>
+      </c>
+      <c r="M16" s="4">
         <v>1128177.3423101599</v>
       </c>
-      <c r="N16">
+      <c r="N16" s="4">
         <v>1080209.0009629901</v>
       </c>
-      <c r="O16">
+      <c r="O16" s="3">
         <f t="shared" si="1"/>
         <v>-13.08105812192639</v>
       </c>
-      <c r="P16">
+      <c r="P16" s="3">
         <f t="shared" si="2"/>
         <v>21.505405474573511</v>
       </c>
-      <c r="Q16">
+      <c r="Q16" s="3">
         <f t="shared" si="3"/>
-        <v>13.146552364966267</v>
+        <v>9.8883014532495874</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="3">
         <v>0.33990975034846399</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="3">
         <v>1.7852728050151801E-2</v>
       </c>
-      <c r="D17">
-        <v>5.7338007280782898E-8</v>
-      </c>
-      <c r="E17">
-        <v>3.0358822738769202E-7</v>
-      </c>
-      <c r="F17">
+      <c r="D17" s="3">
+        <v>0</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0</v>
+      </c>
+      <c r="F17" s="3">
         <v>0.34001470902785202</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="3">
         <v>1.9215267120423499E-2</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="4">
         <v>516093.26919917698</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="4">
         <v>5880.5732883260198</v>
       </c>
-      <c r="J17">
-        <v>0.100000000050186</v>
-      </c>
-      <c r="K17">
-        <v>0.100000000874439</v>
-      </c>
-      <c r="L17">
+      <c r="J17" s="1">
+        <v>0</v>
+      </c>
+      <c r="K17" s="1">
+        <v>0</v>
+      </c>
+      <c r="L17" s="4">
         <f t="shared" si="0"/>
-        <v>521974.0424875039</v>
-      </c>
-      <c r="M17">
+        <v>521973.84248750302</v>
+      </c>
+      <c r="M17" s="4">
         <v>1096283.1583023299</v>
       </c>
-      <c r="N17">
+      <c r="N17" s="4">
         <v>1032964.8558376801</v>
       </c>
-      <c r="O17">
+      <c r="O17" s="3">
         <f t="shared" si="1"/>
         <v>-15.538303647127714</v>
       </c>
-      <c r="P17">
+      <c r="P17" s="3">
         <f t="shared" si="2"/>
         <v>34.047414391175508</v>
       </c>
-      <c r="Q17">
+      <c r="Q17" s="3">
         <f t="shared" si="3"/>
-        <v>24.680589822859702</v>
+        <v>21.090201058665112</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="3">
         <v>0.63706111229470697</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="3">
         <v>1.7852728050151801E-2</v>
       </c>
-      <c r="D18">
-        <v>5.8254042882155698E-8</v>
-      </c>
-      <c r="E18">
-        <v>3.0381735960221701E-7</v>
-      </c>
-      <c r="F18">
+      <c r="D18" s="3">
+        <v>0</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0</v>
+      </c>
+      <c r="F18" s="3">
         <v>0.63716607155178995</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="3">
         <v>2.0406093448743699E-2</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="4">
         <v>806979.19427789305</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="4">
         <v>5876.1382913223797</v>
       </c>
-      <c r="J18">
-        <v>0.10000000009903701</v>
-      </c>
-      <c r="K18">
-        <v>0.100000000857677</v>
-      </c>
-      <c r="L18">
+      <c r="J18" s="1">
+        <v>0</v>
+      </c>
+      <c r="K18" s="1">
+        <v>0</v>
+      </c>
+      <c r="L18" s="4">
         <f t="shared" si="0"/>
-        <v>812855.53256921645</v>
-      </c>
-      <c r="M18">
+        <v>812855.33256921545</v>
+      </c>
+      <c r="M18" s="4">
         <v>899822.95821229403</v>
       </c>
-      <c r="N18">
+      <c r="N18" s="4">
         <v>780246.97689519799</v>
       </c>
-      <c r="O18">
+      <c r="O18" s="3">
         <f t="shared" si="1"/>
         <v>-30.674321782374001</v>
       </c>
-      <c r="P18">
+      <c r="P18" s="3">
         <f t="shared" si="2"/>
         <v>109.60063018895532</v>
       </c>
-      <c r="Q18">
+      <c r="Q18" s="3">
         <f t="shared" si="3"/>
-        <v>94.16158466142673</v>
+        <v>88.570398821797198</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="3">
         <v>0.835052393399349</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="3">
         <v>1.7852728050151801E-2</v>
       </c>
-      <c r="D19">
-        <v>5.8853452252163703E-8</v>
-      </c>
-      <c r="E19">
-        <v>3.0396726463217898E-7</v>
-      </c>
-      <c r="F19">
+      <c r="D19" s="3">
+        <v>0</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0</v>
+      </c>
+      <c r="F19" s="3">
         <v>0.83515735303444705</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="3">
         <v>2.1199538327136801E-2</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="4">
         <v>952896.45011902205</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="4">
         <v>5873.2403952679597</v>
       </c>
-      <c r="J19">
-        <v>0.100000000097707</v>
-      </c>
-      <c r="K19">
-        <v>0.10000000069802401</v>
-      </c>
-      <c r="L19">
+      <c r="J19" s="1">
+        <v>0</v>
+      </c>
+      <c r="K19" s="1">
+        <v>0</v>
+      </c>
+      <c r="L19" s="4">
         <f t="shared" si="0"/>
-        <v>958769.89051429078</v>
-      </c>
-      <c r="M19">
+        <v>958769.69051429001</v>
+      </c>
+      <c r="M19" s="4">
         <v>799832.90192336496</v>
       </c>
-      <c r="N19">
+      <c r="N19" s="4">
         <v>671141.43824272405</v>
       </c>
-      <c r="O19">
+      <c r="O19" s="3">
         <f t="shared" si="1"/>
         <v>-38.377924367731886</v>
       </c>
-      <c r="P19">
+      <c r="P19" s="3">
         <f t="shared" si="2"/>
         <v>147.50042859343756</v>
       </c>
-      <c r="Q19">
+      <c r="Q19" s="3">
         <f t="shared" si="3"/>
-        <v>129.01521095578653</v>
+        <v>122.4203688829658</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="3">
         <v>2.03321156561612E-2</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="3">
         <v>1.7852728050151801E-2</v>
       </c>
-      <c r="D20">
-        <v>5.6327115575681402E-8</v>
-      </c>
-      <c r="E20">
-        <v>3.03335911592695E-7</v>
-      </c>
-      <c r="F20">
+      <c r="D20" s="3">
+        <v>0</v>
+      </c>
+      <c r="E20" s="3">
+        <v>0</v>
+      </c>
+      <c r="F20" s="3">
         <v>2.0437073698036299E-2</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="3">
         <v>1.7934568057712999E-2</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="4">
         <v>39066.798006998099</v>
       </c>
-      <c r="I20">
+      <c r="I20" s="4">
         <v>5885.4647692060998</v>
       </c>
-      <c r="J20">
-        <v>0.100000000051232</v>
-      </c>
-      <c r="K20">
-        <v>0.10000000089054401</v>
-      </c>
-      <c r="L20">
+      <c r="J20" s="1">
+        <v>0</v>
+      </c>
+      <c r="K20" s="1">
+        <v>0</v>
+      </c>
+      <c r="L20" s="4">
         <f t="shared" si="0"/>
-        <v>44952.462776205139</v>
-      </c>
-      <c r="M20">
+        <v>44952.262776204196</v>
+      </c>
+      <c r="M20" s="4">
         <v>1399773.18156359</v>
       </c>
-      <c r="N20">
+      <c r="N20" s="4">
         <v>1579378.15253031</v>
       </c>
-      <c r="O20">
+      <c r="O20" s="3">
         <f t="shared" si="1"/>
         <v>7.8436866686895943</v>
       </c>
-      <c r="P20">
+      <c r="P20" s="3">
         <f t="shared" si="2"/>
         <v>-89.852990585390927</v>
       </c>
-      <c r="Q20">
+      <c r="Q20" s="3">
         <f t="shared" si="3"/>
-        <v>-89.262493693713552</v>
+        <v>-89.571740775989483</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update stf and SAG code
</commit_message>
<xml_diff>
--- a/NSAS/results/stf/NSAS_stf_2020_tab.xlsx
+++ b/NSAS/results/stf/NSAS_stf_2020_tab.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\wg_HAWG\NSAS\results\stf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{02170B20-016B-4E0F-8408-A350FEEB7AFE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6AB1B463-1EF1-4156-A9BD-26AD0928F129}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13725" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t>Fbar 2-6 A</t>
   </si>
@@ -61,9 +61,6 @@
     <t>NA</t>
   </si>
   <si>
-    <t>fmsyAR</t>
-  </si>
-  <si>
     <t>fmsyAR_transfer</t>
   </si>
   <si>
@@ -125,12 +122,27 @@
   </si>
   <si>
     <t>advice change</t>
+  </si>
+  <si>
+    <t>fmsyAR_transfer_Btarget</t>
+  </si>
+  <si>
+    <t>fmsyAR_no_transfer_Btarget</t>
+  </si>
+  <si>
+    <t>fmsyAR_transfer_sq TAC C&amp;D</t>
+  </si>
+  <si>
+    <t>fmsyAR_no_transfer_sq TAC C&amp;D</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.000"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -267,7 +279,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -450,6 +462,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -629,13 +647,15 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -991,18 +1011,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U20"/>
+  <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S9" sqref="S9"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="11" width="12" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" customWidth="1"/>
-    <col min="13" max="14" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="8" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="13.5703125" bestFit="1" customWidth="1"/>
@@ -1041,7 +1061,7 @@
         <v>9</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M1" s="2" t="s">
         <v>10</v>
@@ -1050,63 +1070,63 @@
         <v>10</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="Q1" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="S1" t="s">
+        <v>28</v>
+      </c>
+      <c r="U1" t="s">
         <v>29</v>
-      </c>
-      <c r="U1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="3">
-        <v>0.18971109671771</v>
+        <v>0.196872216327869</v>
       </c>
       <c r="C2" s="3">
-        <v>1.7852728050151801E-2</v>
-      </c>
-      <c r="D2" s="3">
-        <v>0</v>
-      </c>
-      <c r="E2" s="3">
-        <v>0</v>
+        <v>1.7872154284830501E-2</v>
+      </c>
+      <c r="D2" s="5">
+        <v>1.9674353129063302E-3</v>
+      </c>
+      <c r="E2" s="5">
+        <v>7.6751214823222796E-4</v>
       </c>
       <c r="F2" s="3">
-        <v>0.18981601755250199</v>
+        <v>0.198219627163815</v>
       </c>
       <c r="G2" s="3">
-        <v>1.8612989801510001E-2</v>
+        <v>2.1396061256471501E-2</v>
       </c>
       <c r="H2" s="4">
-        <v>379123.90926072001</v>
+        <v>391200.47793567099</v>
       </c>
       <c r="I2" s="4">
-        <v>5614.9800130160002</v>
-      </c>
-      <c r="J2" s="1">
-        <v>0</v>
-      </c>
-      <c r="K2" s="1">
-        <v>0</v>
+        <v>5614.9800130171297</v>
+      </c>
+      <c r="J2" s="4">
+        <v>3330.3937383375501</v>
+      </c>
+      <c r="K2" s="4">
+        <v>241.132954840797</v>
       </c>
       <c r="L2" s="4">
         <f>SUM(H2:K2)</f>
-        <v>384738.88927373604</v>
-      </c>
-      <c r="M2" s="4">
-        <v>1297964.88306625</v>
-      </c>
-      <c r="N2" s="4" t="s">
+        <v>400386.98464186647</v>
+      </c>
+      <c r="M2" s="1">
+        <v>1288877.0345384199</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="O2" s="1"/>
@@ -1120,1029 +1140,1200 @@
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="3">
-        <v>0.22181704827454199</v>
+        <v>0.216325017801619</v>
       </c>
       <c r="C3" s="3">
-        <v>1.7852728050151801E-2</v>
-      </c>
-      <c r="D3" s="3">
-        <v>0</v>
-      </c>
-      <c r="E3" s="3">
+        <v>1.7871964000208001E-2</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4">
         <v>0</v>
       </c>
       <c r="F3" s="3">
-        <v>0.22192200672047599</v>
+        <v>0.21643005661762499</v>
       </c>
       <c r="G3" s="3">
-        <v>1.8742013691114601E-2</v>
+        <v>1.8738899038611399E-2</v>
       </c>
       <c r="H3" s="4">
-        <v>365422.11410823499</v>
+        <v>354086.21211936203</v>
       </c>
       <c r="I3" s="4">
-        <v>5882.3656761106504</v>
-      </c>
-      <c r="J3" s="1">
-        <v>0</v>
-      </c>
-      <c r="K3" s="1">
+        <v>5751.7135261173398</v>
+      </c>
+      <c r="J3" s="4">
+        <v>0</v>
+      </c>
+      <c r="K3" s="4">
         <v>0</v>
       </c>
       <c r="L3" s="4">
-        <f t="shared" ref="L3:L20" si="0">SUM(H3:K3)</f>
-        <v>371304.47978434566</v>
-      </c>
-      <c r="M3" s="4">
-        <v>1194964.6515718</v>
-      </c>
-      <c r="N3" s="4">
-        <v>1185994.5596193699</v>
+        <f t="shared" ref="L3:L23" si="0">SUM(H3:K3)</f>
+        <v>359837.92564547935</v>
+      </c>
+      <c r="M3" s="1">
+        <v>1190399.41122308</v>
+      </c>
+      <c r="N3" s="1">
+        <v>1187591.36299551</v>
       </c>
       <c r="O3" s="3">
         <f>(M3-$M$2)*100/$M$2</f>
-        <v>-7.9355175812713208</v>
+        <v>-7.6405755302023275</v>
       </c>
       <c r="P3" s="3">
         <f>(H3-$S$2)*100/$S$2</f>
-        <v>-5.0871373820193364</v>
+        <v>-8.0314663281381087</v>
       </c>
       <c r="Q3" s="3">
         <f>(L3-$U$2)*100/$U$2</f>
-        <v>-13.862859685069511</v>
+        <v>-16.522930426370369</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>14</v>
+      <c r="A4" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="B4" s="3">
-        <v>0.21779818792893199</v>
+        <v>0.216145764211673</v>
       </c>
       <c r="C4" s="3">
-        <v>1.78525402540128E-2</v>
-      </c>
-      <c r="D4" s="3">
-        <v>0</v>
-      </c>
-      <c r="E4" s="3">
+        <v>4.9117289133332603E-2</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4">
         <v>0</v>
       </c>
       <c r="F4" s="3">
-        <v>0.217903113165408</v>
+        <v>0.21643443240523</v>
       </c>
       <c r="G4" s="3">
-        <v>1.8725379656635399E-2</v>
+        <v>4.9983506017612998E-2</v>
       </c>
       <c r="H4" s="4">
-        <v>359837.45067426999</v>
+        <v>353817.26844644698</v>
       </c>
       <c r="I4" s="4">
-        <v>5882.3666515391096</v>
-      </c>
-      <c r="J4" s="1">
-        <v>0</v>
-      </c>
-      <c r="K4" s="1">
+        <v>15556.950772272499</v>
+      </c>
+      <c r="J4" s="4">
+        <v>0</v>
+      </c>
+      <c r="K4" s="4">
         <v>0</v>
       </c>
       <c r="L4" s="4">
         <f t="shared" si="0"/>
-        <v>365719.8173258091</v>
-      </c>
-      <c r="M4" s="4">
-        <v>1198573.82186475</v>
-      </c>
-      <c r="N4" s="4">
-        <v>1191992.4844736301</v>
+        <v>369374.21921871946</v>
+      </c>
+      <c r="M4" s="1">
+        <v>1190399.8156393501</v>
+      </c>
+      <c r="N4" s="1">
+        <v>1184768.52256763</v>
       </c>
       <c r="O4" s="3">
-        <f t="shared" ref="O4:O20" si="1">(M4-$M$2)*100/$M$2</f>
-        <v>-7.6574537954141961</v>
+        <f t="shared" ref="O4:O23" si="1">(M4-$M$2)*100/$M$2</f>
+        <v>-7.6405441527893352</v>
       </c>
       <c r="P4" s="3">
         <f t="shared" ref="P4:P20" si="2">(H4-$S$2)*100/$S$2</f>
-        <v>-6.5376691719990259</v>
+        <v>-8.1013203760838799</v>
       </c>
       <c r="Q4" s="3">
         <f t="shared" ref="Q4:Q20" si="3">(L4-$U$2)*100/$U$2</f>
-        <v>-15.158418666964591</v>
+        <v>-14.310651549262181</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>15</v>
+      <c r="A5" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="B5" s="3">
-        <v>0.22181707471637299</v>
+        <v>0.21632497736267101</v>
       </c>
       <c r="C5" s="3">
-        <v>1.7852728050151801E-2</v>
-      </c>
-      <c r="D5" s="3">
-        <v>0</v>
-      </c>
-      <c r="E5" s="3">
+        <v>1.7871963998847499E-2</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4">
         <v>0</v>
       </c>
       <c r="F5" s="3">
-        <v>0.22192200651493901</v>
+        <v>0.216430021059071</v>
       </c>
       <c r="G5" s="3">
-        <v>1.8741681696794001E-2</v>
+        <v>1.8738906631995001E-2</v>
       </c>
       <c r="H5" s="4">
-        <v>365422.15330593003</v>
+        <v>354086.15574900003</v>
       </c>
       <c r="I5" s="4">
-        <v>5882.36663649207</v>
-      </c>
-      <c r="J5" s="1">
-        <v>0</v>
-      </c>
-      <c r="K5" s="1">
+        <v>5751.7135127741003</v>
+      </c>
+      <c r="J5" s="4">
+        <v>0</v>
+      </c>
+      <c r="K5" s="4">
         <v>0</v>
       </c>
       <c r="L5" s="4">
         <f t="shared" si="0"/>
-        <v>371304.51994242211</v>
-      </c>
-      <c r="M5" s="4">
-        <v>1194964.65046505</v>
-      </c>
-      <c r="N5" s="4">
-        <v>1185994.6358368699</v>
+        <v>359837.86926177412</v>
+      </c>
+      <c r="M5" s="1">
+        <v>1190399.4431845399</v>
+      </c>
+      <c r="N5" s="1">
+        <v>1187591.40644058</v>
       </c>
       <c r="O5" s="3">
         <f t="shared" si="1"/>
-        <v>-7.9355176665394209</v>
+        <v>-7.6405730504110796</v>
       </c>
       <c r="P5" s="3">
         <f t="shared" si="2"/>
-        <v>-5.0871272010114001</v>
+        <v>-8.031480969486342</v>
       </c>
       <c r="Q5" s="3">
         <f t="shared" si="3"/>
-        <v>-13.862850368990514</v>
+        <v>-16.522943506554945</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>16</v>
+      <c r="A6" s="6" t="s">
+        <v>35</v>
       </c>
       <c r="B6" s="3">
-        <v>0.187751807871259</v>
+        <v>0.216145723891148</v>
       </c>
       <c r="C6" s="3">
-        <v>4.0114451342223897E-2</v>
-      </c>
-      <c r="D6" s="3">
-        <v>0</v>
-      </c>
-      <c r="E6" s="3">
+        <v>4.9117281387116303E-2</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0</v>
+      </c>
+      <c r="E6" s="4">
         <v>0</v>
       </c>
       <c r="F6" s="3">
-        <v>0.18798756125831501</v>
+        <v>0.216434396931006</v>
       </c>
       <c r="G6" s="3">
-        <v>4.08668610889978E-2</v>
+        <v>4.9983505884772503E-2</v>
       </c>
       <c r="H6" s="4">
-        <v>317015.27061757201</v>
+        <v>353817.212233903</v>
       </c>
       <c r="I6" s="4">
-        <v>13067.6949647089</v>
-      </c>
-      <c r="J6" s="1">
-        <v>0</v>
-      </c>
-      <c r="K6" s="1">
+        <v>15556.9483446789</v>
+      </c>
+      <c r="J6" s="4">
+        <v>0</v>
+      </c>
+      <c r="K6" s="4">
         <v>0</v>
       </c>
       <c r="L6" s="4">
         <f t="shared" si="0"/>
-        <v>330082.96558228089</v>
-      </c>
-      <c r="M6" s="4">
-        <v>1226005.83428234</v>
-      </c>
-      <c r="N6" s="4">
-        <v>1236553.1542724799</v>
+        <v>369374.16057858191</v>
+      </c>
+      <c r="M6" s="1">
+        <v>1190399.84753384</v>
+      </c>
+      <c r="N6" s="1">
+        <v>1184768.5666493301</v>
       </c>
       <c r="O6" s="3">
         <f t="shared" si="1"/>
-        <v>-5.5439904209054864</v>
+        <v>-7.6405416781940847</v>
       </c>
       <c r="P6" s="3">
         <f t="shared" si="2"/>
-        <v>-17.660082227493451</v>
+        <v>-8.1013349764412688</v>
       </c>
       <c r="Q6" s="3">
         <f t="shared" si="3"/>
-        <v>-23.425640492021824</v>
+        <v>-14.310665152905635</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>17</v>
+      <c r="A7" s="6" t="s">
+        <v>15</v>
       </c>
       <c r="B7" s="3">
-        <v>0.187751807871259</v>
+        <v>0.18643910667452801</v>
       </c>
       <c r="C7" s="3">
-        <v>4.0114451342223897E-2</v>
-      </c>
-      <c r="D7" s="3">
-        <v>0</v>
-      </c>
-      <c r="E7" s="3">
+        <v>3.9833983852838199E-2</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0</v>
+      </c>
+      <c r="E7" s="4">
         <v>0</v>
       </c>
       <c r="F7" s="3">
-        <v>0.18798756125831501</v>
+        <v>0.18667321174886001</v>
       </c>
       <c r="G7" s="3">
-        <v>4.08668610889978E-2</v>
+        <v>4.0581132988882301E-2</v>
       </c>
       <c r="H7" s="4">
-        <v>317015.27061757201</v>
+        <v>311829.85618844797</v>
       </c>
       <c r="I7" s="4">
-        <v>13067.6949647089</v>
-      </c>
-      <c r="J7" s="1">
-        <v>0</v>
-      </c>
-      <c r="K7" s="1">
+        <v>12677.3824345062</v>
+      </c>
+      <c r="J7" s="4">
+        <v>0</v>
+      </c>
+      <c r="K7" s="4">
         <v>0</v>
       </c>
       <c r="L7" s="4">
         <f t="shared" si="0"/>
-        <v>330082.96558228089</v>
-      </c>
-      <c r="M7" s="4">
-        <v>1226005.83428234</v>
-      </c>
-      <c r="N7" s="4">
-        <v>1236553.1542724799</v>
+        <v>324507.23862295417</v>
+      </c>
+      <c r="M7" s="1">
+        <v>1217433.9896664701</v>
+      </c>
+      <c r="N7" s="1">
+        <v>1231684.1438629201</v>
       </c>
       <c r="O7" s="3">
         <f t="shared" si="1"/>
-        <v>-5.5439904209054864</v>
+        <v>-5.5430458420368565</v>
       </c>
       <c r="P7" s="3">
         <f t="shared" si="2"/>
-        <v>-17.660082227493451</v>
+        <v>-19.006915132036745</v>
       </c>
       <c r="Q7" s="3">
         <f t="shared" si="3"/>
-        <v>-23.425640492021824</v>
+        <v>-24.719126570434376</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>18</v>
+      <c r="A8" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="B8" s="3">
-        <v>0.187751807871259</v>
+        <v>0.18643910667452801</v>
       </c>
       <c r="C8" s="3">
-        <v>4.0114451342223897E-2</v>
-      </c>
-      <c r="D8" s="3">
-        <v>0</v>
-      </c>
-      <c r="E8" s="3">
+        <v>3.9833983852838199E-2</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0</v>
+      </c>
+      <c r="E8" s="4">
         <v>0</v>
       </c>
       <c r="F8" s="3">
-        <v>0.18798756125831501</v>
+        <v>0.18667321174886001</v>
       </c>
       <c r="G8" s="3">
-        <v>4.08668610889978E-2</v>
+        <v>4.0581132988882301E-2</v>
       </c>
       <c r="H8" s="4">
-        <v>317015.27061757201</v>
+        <v>311829.85618844797</v>
       </c>
       <c r="I8" s="4">
-        <v>13067.6949647089</v>
-      </c>
-      <c r="J8" s="1">
-        <v>0</v>
-      </c>
-      <c r="K8" s="1">
+        <v>12677.3824345062</v>
+      </c>
+      <c r="J8" s="4">
+        <v>0</v>
+      </c>
+      <c r="K8" s="4">
         <v>0</v>
       </c>
       <c r="L8" s="4">
         <f t="shared" si="0"/>
-        <v>330082.96558228089</v>
-      </c>
-      <c r="M8" s="4">
-        <v>1226005.83428234</v>
-      </c>
-      <c r="N8" s="4">
-        <v>1236553.1542724799</v>
+        <v>324507.23862295417</v>
+      </c>
+      <c r="M8" s="1">
+        <v>1217433.9896664701</v>
+      </c>
+      <c r="N8" s="1">
+        <v>1231684.1438629201</v>
       </c>
       <c r="O8" s="3">
         <f t="shared" si="1"/>
-        <v>-5.5439904209054864</v>
+        <v>-5.5430458420368565</v>
       </c>
       <c r="P8" s="3">
         <f t="shared" si="2"/>
-        <v>-17.660082227493451</v>
+        <v>-19.006915132036745</v>
       </c>
       <c r="Q8" s="3">
         <f t="shared" si="3"/>
-        <v>-23.425640492021824</v>
+        <v>-24.719126570434376</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>19</v>
+      <c r="A9" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="B9" s="3">
-        <v>0.191772865490872</v>
+        <v>0.18643910667452801</v>
       </c>
       <c r="C9" s="3">
-        <v>4.92314759852484E-2</v>
-      </c>
-      <c r="D9" s="3">
-        <v>0</v>
-      </c>
-      <c r="E9" s="3">
+        <v>3.9833983852838199E-2</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4">
         <v>0</v>
       </c>
       <c r="F9" s="3">
-        <v>0.19206219980369299</v>
+        <v>0.18667321174886001</v>
       </c>
       <c r="G9" s="3">
-        <v>0.05</v>
+        <v>4.0581132988882301E-2</v>
       </c>
       <c r="H9" s="4">
-        <v>322848.82893140498</v>
+        <v>311829.85618844797</v>
       </c>
       <c r="I9" s="4">
-        <v>15962.7127511822</v>
-      </c>
-      <c r="J9" s="1">
-        <v>0</v>
-      </c>
-      <c r="K9" s="1">
+        <v>12677.3824345062</v>
+      </c>
+      <c r="J9" s="4">
+        <v>0</v>
+      </c>
+      <c r="K9" s="4">
         <v>0</v>
       </c>
       <c r="L9" s="4">
         <f t="shared" si="0"/>
-        <v>338811.54168258718</v>
-      </c>
-      <c r="M9" s="4">
-        <v>1222213.99875077</v>
-      </c>
-      <c r="N9" s="4">
-        <v>1229184.5031472701</v>
+        <v>324507.23862295417</v>
+      </c>
+      <c r="M9" s="1">
+        <v>1217433.9896664701</v>
+      </c>
+      <c r="N9" s="1">
+        <v>1231684.1438629201</v>
       </c>
       <c r="O9" s="3">
         <f t="shared" si="1"/>
-        <v>-5.8361274102061804</v>
+        <v>-5.5430458420368565</v>
       </c>
       <c r="P9" s="3">
         <f t="shared" si="2"/>
-        <v>-16.144903760076421</v>
+        <v>-19.006915132036745</v>
       </c>
       <c r="Q9" s="3">
         <f t="shared" si="3"/>
-        <v>-21.400740106391385</v>
+        <v>-24.719126570434376</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>20</v>
+      <c r="A10" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="B10" s="3">
-        <v>0.25990373921313498</v>
+        <v>0.19043479099904201</v>
       </c>
       <c r="C10" s="3">
-        <v>1.7852728050151801E-2</v>
-      </c>
-      <c r="D10" s="3">
-        <v>0</v>
-      </c>
-      <c r="E10" s="3">
+        <v>4.9236838278682603E-2</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0</v>
+      </c>
+      <c r="E10" s="4">
         <v>0</v>
       </c>
       <c r="F10" s="3">
-        <v>0.26000869773462099</v>
+        <v>0.190724156826164</v>
       </c>
       <c r="G10" s="3">
-        <v>1.88946451140619E-2</v>
+        <v>4.99999999999843E-2</v>
       </c>
       <c r="H10" s="4">
-        <v>416773.02872596902</v>
+        <v>317579.78506028099</v>
       </c>
       <c r="I10" s="4">
-        <v>5881.7856979930102</v>
-      </c>
-      <c r="J10" s="1">
-        <v>0</v>
-      </c>
-      <c r="K10" s="1">
+        <v>15594.9451909913</v>
+      </c>
+      <c r="J10" s="4">
+        <v>0</v>
+      </c>
+      <c r="K10" s="4">
         <v>0</v>
       </c>
       <c r="L10" s="4">
         <f t="shared" si="0"/>
-        <v>422654.81442396203</v>
-      </c>
-      <c r="M10" s="4">
-        <v>1161612.8442795801</v>
-      </c>
-      <c r="N10" s="4">
-        <v>1131960.88206297</v>
+        <v>333174.73025127227</v>
+      </c>
+      <c r="M10" s="1">
+        <v>1213699.1798028599</v>
+      </c>
+      <c r="N10" s="1">
+        <v>1224366.0458871401</v>
       </c>
       <c r="O10" s="3">
         <f t="shared" si="1"/>
-        <v>-10.505063778348028</v>
+        <v>-5.8328182379697022</v>
       </c>
       <c r="P10" s="3">
         <f t="shared" si="2"/>
-        <v>8.2504853732828991</v>
+        <v>-17.513458146251249</v>
       </c>
       <c r="Q10" s="3">
         <f t="shared" si="3"/>
-        <v>-1.9503425437728144</v>
+        <v>-22.708396877648166</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>21</v>
+      <c r="A11" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="B11" s="3">
-        <v>0</v>
+        <v>0.259899355637777</v>
       </c>
       <c r="C11" s="3">
-        <v>0</v>
-      </c>
-      <c r="D11" s="3">
-        <v>0</v>
-      </c>
-      <c r="E11" s="3">
+        <v>1.7872154284830501E-2</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4">
         <v>0</v>
       </c>
       <c r="F11" s="3">
-        <v>0</v>
+        <v>0.260004428481936</v>
       </c>
       <c r="G11" s="3">
-        <v>0</v>
+        <v>1.8914061193787898E-2</v>
       </c>
       <c r="H11" s="4">
-        <v>0</v>
+        <v>412493.65816959197</v>
       </c>
       <c r="I11" s="4">
-        <v>0</v>
-      </c>
-      <c r="J11" s="1">
-        <v>0</v>
-      </c>
-      <c r="K11" s="1">
+        <v>5751.1109208400003</v>
+      </c>
+      <c r="J11" s="4">
+        <v>0</v>
+      </c>
+      <c r="K11" s="4">
         <v>0</v>
       </c>
       <c r="L11" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M11" s="4">
-        <v>1423553.23179569</v>
-      </c>
-      <c r="N11" s="4">
-        <v>1634511.7064158299</v>
+        <v>418244.76909043198</v>
+      </c>
+      <c r="M11" s="1">
+        <v>1152527.90615043</v>
+      </c>
+      <c r="N11" s="1">
+        <v>1125890.0735088701</v>
       </c>
       <c r="O11" s="3">
         <f t="shared" si="1"/>
-        <v>9.675789412172394</v>
+        <v>-10.57890898310715</v>
       </c>
       <c r="P11" s="3">
         <f t="shared" si="2"/>
-        <v>-100</v>
+        <v>7.1389836495844179</v>
       </c>
       <c r="Q11" s="3">
         <f t="shared" si="3"/>
-        <v>-100</v>
+        <v>-2.9734077486691066</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>22</v>
+      <c r="A12" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="B12" s="3">
-        <v>0.23609928629001101</v>
+        <v>0</v>
       </c>
       <c r="C12" s="3">
-        <v>1.7852728050151801E-2</v>
-      </c>
-      <c r="D12" s="3">
-        <v>0</v>
-      </c>
-      <c r="E12" s="3">
+        <v>0</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0</v>
+      </c>
+      <c r="E12" s="4">
         <v>0</v>
       </c>
       <c r="F12" s="3">
-        <v>0.23620424476430599</v>
+        <v>0</v>
       </c>
       <c r="G12" s="3">
-        <v>1.87992493884011E-2</v>
+        <v>0</v>
       </c>
       <c r="H12" s="4">
-        <v>385008.04999716103</v>
+        <v>0</v>
       </c>
       <c r="I12" s="4">
-        <v>5882.14797418546</v>
-      </c>
-      <c r="J12" s="1">
-        <v>0</v>
-      </c>
-      <c r="K12" s="1">
+        <v>0</v>
+      </c>
+      <c r="J12" s="4">
+        <v>0</v>
+      </c>
+      <c r="K12" s="4">
         <v>0</v>
       </c>
       <c r="L12" s="4">
         <f t="shared" si="0"/>
-        <v>390890.1979713465</v>
-      </c>
-      <c r="M12" s="4">
-        <v>1182278.96423635</v>
-      </c>
-      <c r="N12" s="4">
-        <v>1165149.24192006</v>
+        <v>0</v>
+      </c>
+      <c r="M12" s="1">
+        <v>1411565.2329983099</v>
+      </c>
+      <c r="N12" s="1">
+        <v>1623713.7564216901</v>
       </c>
       <c r="O12" s="3">
         <f t="shared" si="1"/>
-        <v>-8.9128697038866811</v>
+        <v>9.5189994989574593</v>
       </c>
       <c r="P12" s="3">
         <f t="shared" si="2"/>
-        <v>1.298600575211755E-5</v>
+        <v>-100</v>
       </c>
       <c r="Q12" s="3">
         <f t="shared" si="3"/>
-        <v>-9.3192631288894638</v>
+        <v>-100</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
-        <v>-0.15</v>
+      <c r="A13" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="B13" s="3">
-        <v>0.19481112333456399</v>
+        <v>0.239054868595104</v>
       </c>
       <c r="C13" s="3">
-        <v>1.7852728050151801E-2</v>
-      </c>
-      <c r="D13" s="3">
-        <v>0</v>
-      </c>
-      <c r="E13" s="3">
+        <v>1.7872154284830501E-2</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0</v>
+      </c>
+      <c r="E13" s="4">
         <v>0</v>
       </c>
       <c r="F13" s="3">
-        <v>0.19491608172677499</v>
+        <v>0.23915994139787999</v>
       </c>
       <c r="G13" s="3">
-        <v>1.8633788149297201E-2</v>
+        <v>1.8830527453551699E-2</v>
       </c>
       <c r="H13" s="4">
-        <v>327256.84960990603</v>
+        <v>385008.04999747302</v>
       </c>
       <c r="I13" s="4">
-        <v>5882.7780292859497</v>
-      </c>
-      <c r="J13" s="1">
-        <v>0</v>
-      </c>
-      <c r="K13" s="1">
+        <v>5751.4274497340302</v>
+      </c>
+      <c r="J13" s="4">
+        <v>0</v>
+      </c>
+      <c r="K13" s="4">
         <v>0</v>
       </c>
       <c r="L13" s="4">
         <f t="shared" si="0"/>
-        <v>333139.62763919198</v>
-      </c>
-      <c r="M13" s="4">
-        <v>1219557.9099800901</v>
-      </c>
-      <c r="N13" s="4">
-        <v>1227466.4524769201</v>
+        <v>390759.47744720703</v>
+      </c>
+      <c r="M13" s="1">
+        <v>1170397.7813919201</v>
+      </c>
+      <c r="N13" s="1">
+        <v>1154599.99320403</v>
       </c>
       <c r="O13" s="3">
         <f t="shared" si="1"/>
-        <v>-6.0407622817140503</v>
+        <v>-9.1924403935810943</v>
       </c>
       <c r="P13" s="3">
         <f t="shared" si="2"/>
-        <v>-14.999987114577872</v>
+        <v>1.2986086787592786E-5</v>
       </c>
       <c r="Q13" s="3">
         <f t="shared" si="3"/>
-        <v>-22.716540163783403</v>
+        <v>-9.3495883545274161</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
-        <v>0.15</v>
+      <c r="A14" s="7">
+        <v>-0.15</v>
       </c>
       <c r="B14" s="3">
-        <v>0.27999361750339702</v>
+        <v>0.19719300848250801</v>
       </c>
       <c r="C14" s="3">
-        <v>1.7852728050151801E-2</v>
-      </c>
-      <c r="D14" s="3">
-        <v>0</v>
-      </c>
-      <c r="E14" s="3">
+        <v>1.7872154284830501E-2</v>
+      </c>
+      <c r="D14" s="4">
+        <v>0</v>
+      </c>
+      <c r="E14" s="4">
         <v>0</v>
       </c>
       <c r="F14" s="3">
-        <v>0.28009857606463401</v>
+        <v>0.197298081201947</v>
       </c>
       <c r="G14" s="3">
-        <v>1.8975154778387002E-2</v>
+        <v>1.86627671363736E-2</v>
       </c>
       <c r="H14" s="4">
-        <v>442759.24954855797</v>
+        <v>327256.84999999998</v>
       </c>
       <c r="I14" s="4">
-        <v>5881.4805066923</v>
-      </c>
-      <c r="J14" s="1">
-        <v>0</v>
-      </c>
-      <c r="K14" s="1">
+        <v>5752.0647833431703</v>
+      </c>
+      <c r="J14" s="4">
+        <v>0</v>
+      </c>
+      <c r="K14" s="4">
         <v>0</v>
       </c>
       <c r="L14" s="4">
         <f t="shared" si="0"/>
-        <v>448640.73005525029</v>
-      </c>
-      <c r="M14" s="4">
-        <v>1144622.7695116899</v>
-      </c>
-      <c r="N14" s="4">
-        <v>1105370.1353086301</v>
+        <v>333008.91478334315</v>
+      </c>
+      <c r="M14" s="1">
+        <v>1207664.8415220899</v>
+      </c>
+      <c r="N14" s="1">
+        <v>1216820.6691792801</v>
       </c>
       <c r="O14" s="3">
         <f t="shared" si="1"/>
-        <v>-11.81404177841176</v>
+        <v>-6.3010039623690082</v>
       </c>
       <c r="P14" s="3">
         <f t="shared" si="2"/>
-        <v>15.000012869487898</v>
+        <v>-14.999987013256872</v>
       </c>
       <c r="Q14" s="3">
         <f t="shared" si="3"/>
-        <v>4.078005032976761</v>
+        <v>-22.746863610491495</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>23</v>
+      <c r="A15" s="7">
+        <v>0.15</v>
       </c>
       <c r="B15" s="3">
-        <v>0.18971574075929001</v>
+        <v>0.28358518023374102</v>
       </c>
       <c r="C15" s="3">
-        <v>1.7852728050151801E-2</v>
-      </c>
-      <c r="D15" s="3">
-        <v>0</v>
-      </c>
-      <c r="E15" s="3">
+        <v>1.7872154284830501E-2</v>
+      </c>
+      <c r="D15" s="4">
+        <v>0</v>
+      </c>
+      <c r="E15" s="4">
         <v>0</v>
       </c>
       <c r="F15" s="3">
-        <v>0.189820699141349</v>
+        <v>0.28369025312483198</v>
       </c>
       <c r="G15" s="3">
-        <v>1.8613368536124001E-2</v>
+        <v>1.9008981520264999E-2</v>
       </c>
       <c r="H15" s="4">
-        <v>319884.71577490598</v>
+        <v>442759.24937505898</v>
       </c>
       <c r="I15" s="4">
-        <v>5882.8559345601298</v>
-      </c>
-      <c r="J15" s="1">
-        <v>0</v>
-      </c>
-      <c r="K15" s="1">
+        <v>5750.7519044887404</v>
+      </c>
+      <c r="J15" s="4">
+        <v>0</v>
+      </c>
+      <c r="K15" s="4">
         <v>0</v>
       </c>
       <c r="L15" s="4">
         <f t="shared" si="0"/>
-        <v>325767.57170946611</v>
-      </c>
-      <c r="M15" s="4">
-        <v>1224289.06767751</v>
-      </c>
-      <c r="N15" s="4">
-        <v>1235608.89392044</v>
+        <v>448510.00127954769</v>
+      </c>
+      <c r="M15" s="1">
+        <v>1132753.2074140899</v>
+      </c>
+      <c r="N15" s="1">
+        <v>1094932.81641163</v>
       </c>
       <c r="O15" s="3">
         <f t="shared" si="1"/>
-        <v>-5.6762564496114738</v>
+        <v>-12.113166961675438</v>
       </c>
       <c r="P15" s="3">
         <f t="shared" si="2"/>
-        <v>-16.91478728366528</v>
+        <v>15.000012824424163</v>
       </c>
       <c r="Q15" s="3">
         <f t="shared" si="3"/>
-        <v>-24.426747959814108</v>
+        <v>4.0476778930983697</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>24</v>
+      <c r="A16" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="B16" s="3">
-        <v>0.29990655684655998</v>
+        <v>0.198117159478544</v>
       </c>
       <c r="C16" s="3">
-        <v>1.7852728050151801E-2</v>
-      </c>
-      <c r="D16" s="3">
-        <v>0</v>
-      </c>
-      <c r="E16" s="3">
+        <v>1.7872154284830501E-2</v>
+      </c>
+      <c r="D16" s="4">
+        <v>0</v>
+      </c>
+      <c r="E16" s="4">
         <v>0</v>
       </c>
       <c r="F16" s="3">
-        <v>0.30001151544713001</v>
+        <v>0.19822223219982699</v>
       </c>
       <c r="G16" s="3">
-        <v>1.9054955364361099E-2</v>
+        <v>1.8666470647496301E-2</v>
       </c>
       <c r="H16" s="4">
-        <v>467805.53150954598</v>
+        <v>328570.143041706</v>
       </c>
       <c r="I16" s="4">
-        <v>5881.1785008607403</v>
-      </c>
-      <c r="J16" s="1">
-        <v>0</v>
-      </c>
-      <c r="K16" s="1">
+        <v>5752.0506895397903</v>
+      </c>
+      <c r="J16" s="4">
+        <v>0</v>
+      </c>
+      <c r="K16" s="4">
         <v>0</v>
       </c>
       <c r="L16" s="4">
         <f t="shared" si="0"/>
-        <v>473686.71001040674</v>
-      </c>
-      <c r="M16" s="4">
-        <v>1128177.3423101599</v>
-      </c>
-      <c r="N16" s="4">
-        <v>1080209.0009629901</v>
+        <v>334322.19373124582</v>
+      </c>
+      <c r="M16" s="1">
+        <v>1206821.6372517301</v>
+      </c>
+      <c r="N16" s="1">
+        <v>1215376.6620340501</v>
       </c>
       <c r="O16" s="3">
         <f t="shared" si="1"/>
-        <v>-13.08105812192639</v>
+        <v>-6.366425585050167</v>
       </c>
       <c r="P16" s="3">
         <f t="shared" si="2"/>
-        <v>21.505405474573511</v>
+        <v>-14.658879025447263</v>
       </c>
       <c r="Q16" s="3">
         <f t="shared" si="3"/>
-        <v>9.8883014532495874</v>
+        <v>-22.442202344153323</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>25</v>
+      <c r="A17" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="B17" s="3">
-        <v>0.33990975034846399</v>
+        <v>0.29990077748494798</v>
       </c>
       <c r="C17" s="3">
-        <v>1.7852728050151801E-2</v>
-      </c>
-      <c r="D17" s="3">
-        <v>0</v>
-      </c>
-      <c r="E17" s="3">
+        <v>1.7872154284830501E-2</v>
+      </c>
+      <c r="D17" s="4">
+        <v>0</v>
+      </c>
+      <c r="E17" s="4">
         <v>0</v>
       </c>
       <c r="F17" s="3">
-        <v>0.34001470902785202</v>
+        <v>0.30000585040831401</v>
       </c>
       <c r="G17" s="3">
-        <v>1.9215267120423499E-2</v>
+        <v>1.90743658521033E-2</v>
       </c>
       <c r="H17" s="4">
-        <v>516093.26919917698</v>
+        <v>463033.22556123999</v>
       </c>
       <c r="I17" s="4">
-        <v>5880.5732883260198</v>
-      </c>
-      <c r="J17" s="1">
-        <v>0</v>
-      </c>
-      <c r="K17" s="1">
+        <v>5750.5050078332497</v>
+      </c>
+      <c r="J17" s="4">
+        <v>0</v>
+      </c>
+      <c r="K17" s="4">
         <v>0</v>
       </c>
       <c r="L17" s="4">
         <f t="shared" si="0"/>
-        <v>521973.84248750302</v>
-      </c>
-      <c r="M17" s="4">
-        <v>1096283.1583023299</v>
-      </c>
-      <c r="N17" s="4">
-        <v>1032964.8558376801</v>
+        <v>468783.73056907323</v>
+      </c>
+      <c r="M17" s="1">
+        <v>1119450.67142951</v>
+      </c>
+      <c r="N17" s="1">
+        <v>1074573.3527964901</v>
       </c>
       <c r="O17" s="3">
         <f t="shared" si="1"/>
-        <v>-15.538303647127714</v>
+        <v>-13.145269763425171</v>
       </c>
       <c r="P17" s="3">
         <f t="shared" si="2"/>
-        <v>34.047414391175508</v>
+        <v>20.265871244555953</v>
       </c>
       <c r="Q17" s="3">
         <f t="shared" si="3"/>
-        <v>21.090201058665112</v>
+        <v>8.7508828356647612</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>26</v>
+      <c r="A18" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="B18" s="3">
-        <v>0.63706111229470697</v>
+        <v>0.33990238360694902</v>
       </c>
       <c r="C18" s="3">
-        <v>1.7852728050151801E-2</v>
-      </c>
-      <c r="D18" s="3">
-        <v>0</v>
-      </c>
-      <c r="E18" s="3">
+        <v>1.7872154284830501E-2</v>
+      </c>
+      <c r="D18" s="4">
+        <v>0</v>
+      </c>
+      <c r="E18" s="4">
         <v>0</v>
       </c>
       <c r="F18" s="3">
-        <v>0.63716607155178995</v>
+        <v>0.34000745660925502</v>
       </c>
       <c r="G18" s="3">
-        <v>2.0406093448743699E-2</v>
+        <v>1.9234671248370999E-2</v>
       </c>
       <c r="H18" s="4">
-        <v>806979.19427789305</v>
+        <v>510861.81034296099</v>
       </c>
       <c r="I18" s="4">
-        <v>5876.1382913223797</v>
-      </c>
-      <c r="J18" s="1">
-        <v>0</v>
-      </c>
-      <c r="K18" s="1">
+        <v>5749.9010744694197</v>
+      </c>
+      <c r="J18" s="4">
+        <v>0</v>
+      </c>
+      <c r="K18" s="4">
         <v>0</v>
       </c>
       <c r="L18" s="4">
         <f t="shared" si="0"/>
-        <v>812855.33256921545</v>
-      </c>
-      <c r="M18" s="4">
-        <v>899822.95821229403</v>
-      </c>
-      <c r="N18" s="4">
-        <v>780246.97689519799</v>
+        <v>516611.71141743043</v>
+      </c>
+      <c r="M18" s="1">
+        <v>1087895.1724829201</v>
+      </c>
+      <c r="N18" s="1">
+        <v>1027715.37197099</v>
       </c>
       <c r="O18" s="3">
         <f t="shared" si="1"/>
-        <v>-30.674321782374001</v>
+        <v>-15.593563751213598</v>
       </c>
       <c r="P18" s="3">
         <f t="shared" si="2"/>
-        <v>109.60063018895532</v>
+        <v>32.688622143685585</v>
       </c>
       <c r="Q18" s="3">
         <f t="shared" si="3"/>
-        <v>88.570398821797198</v>
+        <v>19.846266063218383</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>27</v>
+      <c r="A19" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="B19" s="3">
-        <v>0.835052393399349</v>
+        <v>0.62542471328373905</v>
       </c>
       <c r="C19" s="3">
-        <v>1.7852728050151801E-2</v>
-      </c>
-      <c r="D19" s="3">
-        <v>0</v>
-      </c>
-      <c r="E19" s="3">
+        <v>1.7872154284830501E-2</v>
+      </c>
+      <c r="D19" s="4">
+        <v>0</v>
+      </c>
+      <c r="E19" s="4">
         <v>0</v>
       </c>
       <c r="F19" s="3">
-        <v>0.83515735303444705</v>
+        <v>0.62552978684226002</v>
       </c>
       <c r="G19" s="3">
-        <v>2.1199538327136801E-2</v>
+        <v>2.0378894545052199E-2</v>
       </c>
       <c r="H19" s="4">
-        <v>952896.45011902205</v>
+        <v>789683.80210091395</v>
       </c>
       <c r="I19" s="4">
-        <v>5873.2403952679597</v>
-      </c>
-      <c r="J19" s="1">
-        <v>0</v>
-      </c>
-      <c r="K19" s="1">
+        <v>5745.6464195618701</v>
+      </c>
+      <c r="J19" s="4">
+        <v>0</v>
+      </c>
+      <c r="K19" s="4">
         <v>0</v>
       </c>
       <c r="L19" s="4">
         <f t="shared" si="0"/>
-        <v>958769.69051429001</v>
-      </c>
-      <c r="M19" s="4">
-        <v>799832.90192336496</v>
-      </c>
-      <c r="N19" s="4">
-        <v>671141.43824272405</v>
+        <v>795429.44852047577</v>
+      </c>
+      <c r="M19" s="1">
+        <v>899911.742305447</v>
+      </c>
+      <c r="N19" s="1">
+        <v>784319.52013662399</v>
       </c>
       <c r="O19" s="3">
         <f t="shared" si="1"/>
-        <v>-38.377924367731886</v>
+        <v>-30.178619201813259</v>
       </c>
       <c r="P19" s="3">
         <f t="shared" si="2"/>
-        <v>147.50042859343756</v>
+        <v>105.10841387735164</v>
       </c>
       <c r="Q19" s="3">
         <f t="shared" si="3"/>
-        <v>122.4203688829658</v>
+        <v>84.527851798691557</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>28</v>
+      <c r="A20" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="B20" s="3">
-        <v>2.03321156561612E-2</v>
+        <v>0.822900368727839</v>
       </c>
       <c r="C20" s="3">
-        <v>1.7852728050151801E-2</v>
-      </c>
-      <c r="D20" s="3">
-        <v>0</v>
-      </c>
-      <c r="E20" s="3">
+        <v>1.7872154284830501E-2</v>
+      </c>
+      <c r="D20" s="4">
+        <v>0</v>
+      </c>
+      <c r="E20" s="4">
         <v>0</v>
       </c>
       <c r="F20" s="3">
-        <v>2.0437073698036299E-2</v>
+        <v>0.82300544266430498</v>
       </c>
       <c r="G20" s="3">
-        <v>1.7934568057712999E-2</v>
+        <v>2.1170273075360398E-2</v>
       </c>
       <c r="H20" s="4">
-        <v>39066.798006998099</v>
+        <v>935833.88392189203</v>
       </c>
       <c r="I20" s="4">
-        <v>5885.4647692060998</v>
-      </c>
-      <c r="J20" s="1">
-        <v>0</v>
-      </c>
-      <c r="K20" s="1">
+        <v>5742.7592398566303</v>
+      </c>
+      <c r="J20" s="4">
+        <v>0</v>
+      </c>
+      <c r="K20" s="4">
         <v>0</v>
       </c>
       <c r="L20" s="4">
         <f t="shared" si="0"/>
-        <v>44952.262776204196</v>
-      </c>
-      <c r="M20" s="4">
-        <v>1399773.18156359</v>
-      </c>
-      <c r="N20" s="4">
-        <v>1579378.15253031</v>
+        <v>941576.64316174865</v>
+      </c>
+      <c r="M20" s="1">
+        <v>799917.64119871799</v>
+      </c>
+      <c r="N20" s="1">
+        <v>674205.97221408295</v>
       </c>
       <c r="O20" s="3">
         <f t="shared" si="1"/>
-        <v>7.8436866686895943</v>
+        <v>-37.9368535738408</v>
       </c>
       <c r="P20" s="3">
         <f t="shared" si="2"/>
-        <v>-89.852990585390927</v>
+        <v>143.06868530573183</v>
       </c>
       <c r="Q20" s="3">
         <f t="shared" si="3"/>
-        <v>-89.571740775989483</v>
+        <v>118.43183652508192</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="3">
+        <v>1.9687221632786899E-9</v>
+      </c>
+      <c r="C21" s="3">
+        <v>1.7872154284830501E-2</v>
+      </c>
+      <c r="D21" s="4">
+        <v>0</v>
+      </c>
+      <c r="E21" s="4">
+        <v>0</v>
+      </c>
+      <c r="F21" s="3">
+        <v>1.05074291255233E-4</v>
+      </c>
+      <c r="G21" s="3">
+        <v>1.78725212757898E-2</v>
+      </c>
+      <c r="H21" s="4">
+        <v>3.8049348238193598E-3</v>
+      </c>
+      <c r="I21" s="4">
+        <v>5755.0972026871896</v>
+      </c>
+      <c r="J21" s="4">
+        <v>0</v>
+      </c>
+      <c r="K21" s="4">
+        <v>0</v>
+      </c>
+      <c r="L21" s="4">
+        <f t="shared" si="0"/>
+        <v>5755.1010076220136</v>
+      </c>
+      <c r="M21" s="1">
+        <v>1411470.78607841</v>
+      </c>
+      <c r="N21" s="1">
+        <v>1621856.6231869301</v>
+      </c>
+      <c r="O21" s="3">
+        <f t="shared" si="1"/>
+        <v>9.5116716532926713</v>
+      </c>
+      <c r="P21" s="3">
+        <f t="shared" ref="P21:P23" si="4">(H21-$S$2)*100/$S$2</f>
+        <v>-99.999999011725777</v>
+      </c>
+      <c r="Q21" s="3">
+        <f t="shared" ref="Q21:Q23" si="5">(L21-$U$2)*100/$U$2</f>
+        <v>-98.664901798900843</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="3">
+        <v>0.223931653013941</v>
+      </c>
+      <c r="C22" s="3">
+        <v>1.7872386610714899E-2</v>
+      </c>
+      <c r="D22" s="5">
+        <v>1.9074359852257099E-3</v>
+      </c>
+      <c r="E22" s="5">
+        <v>7.4999586925621697E-4</v>
+      </c>
+      <c r="F22" s="3">
+        <v>0.22524121207121101</v>
+      </c>
+      <c r="G22" s="3">
+        <v>2.1427217857773701E-2</v>
+      </c>
+      <c r="H22" s="4">
+        <v>364433.03143527498</v>
+      </c>
+      <c r="I22" s="4">
+        <v>5746.1935053015204</v>
+      </c>
+      <c r="J22" s="4">
+        <v>3330.3937334622401</v>
+      </c>
+      <c r="K22" s="4">
+        <v>241.13295480858301</v>
+      </c>
+      <c r="L22" s="4">
+        <f t="shared" si="0"/>
+        <v>373750.75162884739</v>
+      </c>
+      <c r="M22" s="1">
+        <v>1182632.6329943</v>
+      </c>
+      <c r="N22" s="1">
+        <v>1172145.9301903101</v>
+      </c>
+      <c r="O22" s="3">
+        <f t="shared" si="1"/>
+        <v>-8.2431759351014264</v>
+      </c>
+      <c r="P22" s="3">
+        <f t="shared" si="4"/>
+        <v>-5.34403663423228</v>
+      </c>
+      <c r="Q22" s="3">
+        <f t="shared" si="5"/>
+        <v>-13.295360846270981</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" s="3">
+        <v>0.21398473381143199</v>
+      </c>
+      <c r="C23" s="3">
+        <v>1.7871962482682399E-2</v>
+      </c>
+      <c r="D23" s="5">
+        <v>3.8206884672328202E-3</v>
+      </c>
+      <c r="E23" s="5">
+        <v>7.5041015114866104E-4</v>
+      </c>
+      <c r="F23" s="3">
+        <v>0.216498067381413</v>
+      </c>
+      <c r="G23" s="3">
+        <v>2.3300598512852402E-2</v>
+      </c>
+      <c r="H23" s="4">
+        <v>350625.92500995798</v>
+      </c>
+      <c r="I23" s="4">
+        <v>5742.8848952196904</v>
+      </c>
+      <c r="J23" s="4">
+        <v>6660.7874766719997</v>
+      </c>
+      <c r="K23" s="4">
+        <v>241.13295484068999</v>
+      </c>
+      <c r="L23" s="4">
+        <f t="shared" si="0"/>
+        <v>363270.73033669032</v>
+      </c>
+      <c r="M23" s="1">
+        <v>1190466.4826420399</v>
+      </c>
+      <c r="N23" s="1">
+        <v>1182742.7368554</v>
+      </c>
+      <c r="O23" s="3">
+        <f t="shared" si="1"/>
+        <v>-7.6353716653523422</v>
+      </c>
+      <c r="P23" s="3">
+        <f t="shared" si="4"/>
+        <v>-8.9302235252363644</v>
+      </c>
+      <c r="Q23" s="3">
+        <f t="shared" si="5"/>
+        <v>-15.726570577622169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>